<commit_message>
gave lecture 7, added homework 2
</commit_message>
<xml_diff>
--- a/in-class/07/transfer-free-energy.xlsx
+++ b/in-class/07/transfer-free-energy.xlsx
@@ -34,10 +34,10 @@
     <t xml:space="preserve">kJ/mol</t>
   </si>
   <si>
+    <t xml:space="preserve">C/S</t>
+  </si>
+  <si>
     <t xml:space="preserve">N/O</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C/S</t>
   </si>
   <si>
     <t xml:space="preserve">alanine</t>
@@ -240,15 +240,13 @@
   <dimension ref="1:18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="13.5867346938776"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.25"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>